<commit_message>
Add: Adding data into excel file
</commit_message>
<xml_diff>
--- a/MarksList.xlsx
+++ b/MarksList.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -522,6 +522,142 @@
       </c>
       <c r="E6" t="n">
         <v>78</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>A7</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>C7</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>A8</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>B8</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>C8</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>A9</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>B9</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>C9</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>A10</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>B10</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>C10</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>A11</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>B11</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>C11</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>A12</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>B12</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>C12</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>A13</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>B13</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>C13</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>A14</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>B14</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>C14</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: Sheet Properties Accessing
</commit_message>
<xml_diff>
--- a/MarksList.xlsx
+++ b/MarksList.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="NEWSHEET" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -391,6 +392,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor rgb="001d4be5"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -709,4 +711,22 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>